<commit_message>
fixed some stuff on shoot elongation
</commit_message>
<xml_diff>
--- a/data/monitoringShootElongation/2025ShootElongation.xlsx
+++ b/data/monitoringShootElongation/2025ShootElongation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringShootElongation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70DF1D6-A01B-4142-9960-A3EC5A1DC778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EB6F4A-896E-F340-9A2D-4F2E2C12B0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30300" yWindow="-860" windowWidth="29400" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="667">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2021,6 +2021,9 @@
   </si>
   <si>
     <t>doy135: measurement from previous weeks are invalid because shoot snapped off.</t>
+  </si>
+  <si>
+    <t>doy129: dead</t>
   </si>
 </sst>
 </file>
@@ -2521,10 +2524,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3142,9 +3146,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A476" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L486" sqref="L486"/>
+    <sheetView tabSelected="1" topLeftCell="A518" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K486" sqref="K486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17767,7 +17771,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="465" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>487</v>
       </c>
@@ -17790,7 +17794,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="466" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>488</v>
       </c>
@@ -17813,7 +17817,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="467" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>489</v>
       </c>
@@ -17836,7 +17840,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="468" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>490</v>
       </c>
@@ -17859,7 +17863,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="469" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>491</v>
       </c>
@@ -17885,7 +17889,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="470" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>492</v>
       </c>
@@ -17908,7 +17912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="471" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>493</v>
       </c>
@@ -17931,7 +17935,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>494</v>
       </c>
@@ -17954,7 +17958,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="473" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>495</v>
       </c>
@@ -17977,7 +17981,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>496</v>
       </c>
@@ -18000,7 +18004,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>497</v>
       </c>
@@ -18023,7 +18027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="476" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>498</v>
       </c>
@@ -18048,8 +18052,11 @@
       <c r="L476">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="477" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M476" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="477" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>499</v>
       </c>
@@ -18072,7 +18079,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="478" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>500</v>
       </c>
@@ -18095,7 +18102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="479" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>501</v>
       </c>
@@ -18118,7 +18125,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="480" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>502</v>
       </c>
@@ -18157,10 +18164,15 @@
       <c r="E481" t="s">
         <v>460</v>
       </c>
+      <c r="F481" t="s">
+        <v>666</v>
+      </c>
       <c r="K481" t="s">
         <v>649</v>
       </c>
-      <c r="L481" s="2"/>
+      <c r="L481" s="2" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="482" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
@@ -18201,7 +18213,7 @@
       <c r="E483" t="s">
         <v>460</v>
       </c>
-      <c r="K483" s="2">
+      <c r="K483" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="L483">
@@ -18224,7 +18236,7 @@
       <c r="E484" t="s">
         <v>460</v>
       </c>
-      <c r="K484" s="2">
+      <c r="K484" s="3">
         <v>3.9</v>
       </c>
       <c r="L484">
@@ -18247,8 +18259,8 @@
       <c r="E485" t="s">
         <v>460</v>
       </c>
-      <c r="K485" s="2">
-        <v>2.2000000000000002</v>
+      <c r="K485" s="3" t="s">
+        <v>649</v>
       </c>
       <c r="L485">
         <v>3.3</v>
@@ -18270,8 +18282,8 @@
       <c r="E486" t="s">
         <v>460</v>
       </c>
-      <c r="K486" s="2">
-        <v>2.4</v>
+      <c r="K486" s="3" t="s">
+        <v>649</v>
       </c>
       <c r="L486">
         <v>2.1</v>
@@ -18293,7 +18305,9 @@
       <c r="E487" t="s">
         <v>460</v>
       </c>
-      <c r="K487" s="2"/>
+      <c r="K487" s="2">
+        <v>2.4</v>
+      </c>
       <c r="L487">
         <v>2.5</v>
       </c>

</xml_diff>

<commit_message>
phenomonitoring and shoot elongation 142
</commit_message>
<xml_diff>
--- a/data/monitoringShootElongation/2025ShootElongation.xlsx
+++ b/data/monitoringShootElongation/2025ShootElongation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanmeier/TELab/fuelinex/data/monitoringShootElongation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringShootElongation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F2301-8874-D744-A86D-1536E7667EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A74B84-F9CC-254D-A882-CA13ABCCC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="671">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2011,9 +2011,6 @@
     <t>doy128: broke measured shoot. Prior measurements are invalid</t>
   </si>
   <si>
-    <t>doy128: not fully bud bursted. Have not started to elongate yet</t>
-  </si>
-  <si>
     <t>135</t>
   </si>
   <si>
@@ -2033,6 +2030,12 @@
   </si>
   <si>
     <t>doy142: measurement from 135 is probably wrong</t>
+  </si>
+  <si>
+    <t>doy128: not fully bud bursted. Have not started to elongate yet; doy142: apical meristem didn’t budburst, lateral shoot measured</t>
+  </si>
+  <si>
+    <t>doy135: previous measurement (128) is invalid</t>
   </si>
 </sst>
 </file>
@@ -2737,7 +2740,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2832,7 +2835,7 @@
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="betula"/>
+        <filter val="populus"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3175,9 +3178,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M132" sqref="M132"/>
+    <sheetView tabSelected="1" topLeftCell="A312" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O326" sqref="O326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3227,10 +3230,10 @@
         <v>660</v>
       </c>
       <c r="M1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="N1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -7009,7 +7012,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -7037,8 +7040,14 @@
       <c r="L102">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M102">
+        <v>0.4</v>
+      </c>
+      <c r="N102">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -7066,8 +7075,14 @@
       <c r="L103">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M103">
+        <v>3.7</v>
+      </c>
+      <c r="N103">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -7095,8 +7110,14 @@
       <c r="L104">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M104">
+        <v>3.3</v>
+      </c>
+      <c r="N104">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -7124,8 +7145,14 @@
       <c r="L105">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M105">
+        <v>3.8</v>
+      </c>
+      <c r="N105">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -7152,6 +7179,12 @@
       </c>
       <c r="L106">
         <v>6.9</v>
+      </c>
+      <c r="M106">
+        <v>7.3</v>
+      </c>
+      <c r="N106">
+        <v>8.5</v>
       </c>
     </row>
     <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -7504,7 +7537,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -7532,8 +7565,14 @@
       <c r="L117">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M117">
+        <v>2.5</v>
+      </c>
+      <c r="N117">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -7561,8 +7600,14 @@
       <c r="L118">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M118">
+        <v>3.1</v>
+      </c>
+      <c r="N118">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -7590,8 +7635,14 @@
       <c r="L119">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M119">
+        <v>0.6</v>
+      </c>
+      <c r="N119">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -7619,8 +7670,14 @@
       <c r="L120">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M120">
+        <v>3.9</v>
+      </c>
+      <c r="N120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -7646,6 +7703,12 @@
         <v>0.6</v>
       </c>
       <c r="L121">
+        <v>0.6</v>
+      </c>
+      <c r="M121">
+        <v>0.6</v>
+      </c>
+      <c r="N121">
         <v>0.6</v>
       </c>
     </row>
@@ -7999,7 +8062,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -8027,8 +8090,14 @@
       <c r="L132">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M132">
+        <v>2.4</v>
+      </c>
+      <c r="N132">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -8056,8 +8125,14 @@
       <c r="L133">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M133">
+        <v>1.8</v>
+      </c>
+      <c r="N133">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -8085,8 +8160,14 @@
       <c r="L134">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M134">
+        <v>4.3</v>
+      </c>
+      <c r="N134">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -8114,8 +8195,14 @@
       <c r="L135">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M135">
+        <v>1.4</v>
+      </c>
+      <c r="N135">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -8142,6 +8229,12 @@
       </c>
       <c r="L136">
         <v>3.6</v>
+      </c>
+      <c r="M136">
+        <v>3.6</v>
+      </c>
+      <c r="N136">
+        <v>6.9</v>
       </c>
     </row>
     <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8494,7 +8587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -8522,8 +8615,14 @@
       <c r="L147">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M147">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N147">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -8551,8 +8650,14 @@
       <c r="L148">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M148">
+        <v>6.5</v>
+      </c>
+      <c r="N148">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -8580,8 +8685,14 @@
       <c r="L149">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M149">
+        <v>5.5</v>
+      </c>
+      <c r="N149">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -8609,8 +8720,14 @@
       <c r="L150">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M150">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="N150">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -8637,6 +8754,12 @@
       </c>
       <c r="L151">
         <v>0.5</v>
+      </c>
+      <c r="M151">
+        <v>0.5</v>
+      </c>
+      <c r="N151">
+        <v>0.6</v>
       </c>
     </row>
     <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8992,7 +9115,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -9020,8 +9143,14 @@
       <c r="L162">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M162">
+        <v>3.2</v>
+      </c>
+      <c r="N162">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -9049,8 +9178,14 @@
       <c r="L163">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M163">
+        <v>0.5</v>
+      </c>
+      <c r="N163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -9078,8 +9213,14 @@
       <c r="L164">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M164">
+        <v>3.2</v>
+      </c>
+      <c r="N164">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -9107,8 +9248,14 @@
       <c r="L165">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M165">
+        <v>6.6</v>
+      </c>
+      <c r="N165">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -9135,6 +9282,12 @@
       </c>
       <c r="L166">
         <v>2.1</v>
+      </c>
+      <c r="M166">
+        <v>2.9</v>
+      </c>
+      <c r="N166">
+        <v>3.4</v>
       </c>
     </row>
     <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -9487,7 +9640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -9515,8 +9668,14 @@
       <c r="L177">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M177">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N177">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -9544,8 +9703,14 @@
       <c r="L178">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M178">
+        <v>3.6</v>
+      </c>
+      <c r="N178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -9573,8 +9738,14 @@
       <c r="L179">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M179">
+        <v>3.4</v>
+      </c>
+      <c r="N179">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -9602,8 +9773,14 @@
       <c r="L180">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M180">
+        <v>6</v>
+      </c>
+      <c r="N180">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -9630,6 +9807,12 @@
       </c>
       <c r="L181">
         <v>3.4</v>
+      </c>
+      <c r="M181">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N181">
+        <v>4.5</v>
       </c>
     </row>
     <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -11055,7 +11238,7 @@
         <v>198</v>
       </c>
       <c r="F222" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H222">
         <v>1</v>
@@ -11198,7 +11381,7 @@
         <v>198</v>
       </c>
       <c r="F226" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H226">
         <v>0.6</v>
@@ -12534,7 +12717,7 @@
         <v>198</v>
       </c>
       <c r="F264" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H264">
         <v>0.8</v>
@@ -13153,7 +13336,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="282" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>300</v>
       </c>
@@ -13181,8 +13364,14 @@
       <c r="L282">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M282">
+        <v>4.3</v>
+      </c>
+      <c r="N282">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -13210,8 +13399,14 @@
       <c r="L283">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M283">
+        <v>7.3</v>
+      </c>
+      <c r="N283">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>302</v>
       </c>
@@ -13239,8 +13434,14 @@
       <c r="L284">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="285" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M284">
+        <v>5.5</v>
+      </c>
+      <c r="N284">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -13267,6 +13468,12 @@
       </c>
       <c r="L285">
         <v>3.7</v>
+      </c>
+      <c r="M285">
+        <v>13.4</v>
+      </c>
+      <c r="N285">
+        <v>15.8</v>
       </c>
     </row>
     <row r="286" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -13619,7 +13826,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -13647,8 +13854,14 @@
       <c r="L296">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="297" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M296">
+        <v>9.9</v>
+      </c>
+      <c r="N296">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -13676,8 +13889,14 @@
       <c r="L297">
         <v>10.4</v>
       </c>
-    </row>
-    <row r="298" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M297">
+        <v>12.5</v>
+      </c>
+      <c r="N297">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -13705,8 +13924,14 @@
       <c r="L298">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M298">
+        <v>8.4</v>
+      </c>
+      <c r="N298">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -13734,8 +13959,14 @@
       <c r="L299">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M299">
+        <v>15.1</v>
+      </c>
+      <c r="N299">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -13762,6 +13993,12 @@
       </c>
       <c r="L300">
         <v>10.6</v>
+      </c>
+      <c r="M300">
+        <v>13.3</v>
+      </c>
+      <c r="N300">
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -14114,7 +14351,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -14142,8 +14379,14 @@
       <c r="L311">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M311">
+        <v>6</v>
+      </c>
+      <c r="N311">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -14171,8 +14414,14 @@
       <c r="L312">
         <v>2</v>
       </c>
-    </row>
-    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M312">
+        <v>2.5</v>
+      </c>
+      <c r="N312">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -14200,8 +14449,14 @@
       <c r="L313">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="314" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M313">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N313">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -14229,8 +14484,14 @@
       <c r="L314">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M314">
+        <v>6.3</v>
+      </c>
+      <c r="N314">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -14257,6 +14518,12 @@
       </c>
       <c r="L315">
         <v>5.6</v>
+      </c>
+      <c r="M315">
+        <v>6.7</v>
+      </c>
+      <c r="N315">
+        <v>7.1</v>
       </c>
     </row>
     <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -14539,7 +14806,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -14567,8 +14834,14 @@
       <c r="L324">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M324">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="N324">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -14596,8 +14869,14 @@
       <c r="L325">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M325">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N325">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -14628,8 +14907,14 @@
       <c r="L326" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M326" t="s">
+        <v>649</v>
+      </c>
+      <c r="N326" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -14660,8 +14945,14 @@
       <c r="L327" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M327" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="N327" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -14688,6 +14979,12 @@
       </c>
       <c r="L328">
         <v>2.6</v>
+      </c>
+      <c r="M328">
+        <v>3.4</v>
+      </c>
+      <c r="N328">
+        <v>3.9</v>
       </c>
     </row>
     <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -15040,7 +15337,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
@@ -15068,8 +15365,14 @@
       <c r="L339">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="340" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M339">
+        <v>7</v>
+      </c>
+      <c r="N339">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
@@ -15097,8 +15400,14 @@
       <c r="L340">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="341" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M340">
+        <v>6.9</v>
+      </c>
+      <c r="N340">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
@@ -15126,8 +15435,14 @@
       <c r="L341">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M341">
+        <v>3</v>
+      </c>
+      <c r="N341">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
@@ -15158,8 +15473,14 @@
       <c r="L342" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M342" t="s">
+        <v>649</v>
+      </c>
+      <c r="N342" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
@@ -15186,6 +15507,12 @@
       </c>
       <c r="L343">
         <v>4.5999999999999996</v>
+      </c>
+      <c r="M343">
+        <v>5.8</v>
+      </c>
+      <c r="N343">
+        <v>7.1</v>
       </c>
     </row>
     <row r="344" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -15356,10 +15683,10 @@
       <c r="L348">
         <v>15.4</v>
       </c>
-      <c r="M348" s="3">
+      <c r="M348">
         <v>18.399999999999999</v>
       </c>
-      <c r="N348" s="3">
+      <c r="N348">
         <v>20.3</v>
       </c>
     </row>
@@ -15503,7 +15830,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>371</v>
       </c>
@@ -15531,8 +15858,14 @@
       <c r="L353">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M353">
+        <v>15.5</v>
+      </c>
+      <c r="N353">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>372</v>
       </c>
@@ -15560,8 +15893,14 @@
       <c r="L354" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M354">
+        <v>18</v>
+      </c>
+      <c r="N354">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>373</v>
       </c>
@@ -15589,8 +15928,14 @@
       <c r="L355">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M355">
+        <v>13.7</v>
+      </c>
+      <c r="N355">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>374</v>
       </c>
@@ -15618,8 +15963,14 @@
       <c r="L356">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M356">
+        <v>15.2</v>
+      </c>
+      <c r="N356">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>375</v>
       </c>
@@ -15647,8 +15998,14 @@
       <c r="L357">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M357">
+        <v>5.6</v>
+      </c>
+      <c r="N357">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>376</v>
       </c>
@@ -15686,7 +16043,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>379</v>
       </c>
@@ -15724,7 +16081,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>380</v>
       </c>
@@ -15762,7 +16119,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>381</v>
       </c>
@@ -15800,7 +16157,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>382</v>
       </c>
@@ -15838,7 +16195,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>383</v>
       </c>
@@ -15876,7 +16233,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>384</v>
       </c>
@@ -15914,7 +16271,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>385</v>
       </c>
@@ -15952,7 +16309,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>386</v>
       </c>
@@ -15990,7 +16347,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>387</v>
       </c>
@@ -16028,7 +16385,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>388</v>
       </c>
@@ -16805,7 +17162,7 @@
         <v>378</v>
       </c>
       <c r="F388" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G388" s="1">
         <v>3.2</v>
@@ -17457,7 +17814,7 @@
         <v>378</v>
       </c>
       <c r="F405" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G405">
         <v>4.2</v>
@@ -19012,6 +19369,12 @@
       <c r="L448">
         <v>6</v>
       </c>
+      <c r="M448">
+        <v>6.9</v>
+      </c>
+      <c r="N448">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="449" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
@@ -19035,6 +19398,12 @@
       <c r="L449">
         <v>12.1</v>
       </c>
+      <c r="M449">
+        <v>12.1</v>
+      </c>
+      <c r="N449">
+        <v>12.2</v>
+      </c>
     </row>
     <row r="450" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
@@ -19058,6 +19427,12 @@
       <c r="L450">
         <v>5.4</v>
       </c>
+      <c r="M450">
+        <v>7.2</v>
+      </c>
+      <c r="N450">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="451" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
@@ -19081,6 +19456,12 @@
       <c r="L451">
         <v>2</v>
       </c>
+      <c r="M451">
+        <v>2</v>
+      </c>
+      <c r="N451">
+        <v>2</v>
+      </c>
     </row>
     <row r="452" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
@@ -19104,6 +19485,12 @@
       <c r="L452">
         <v>8</v>
       </c>
+      <c r="M452">
+        <v>8.1</v>
+      </c>
+      <c r="N452">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="453" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
@@ -19412,13 +19799,19 @@
         <v>460</v>
       </c>
       <c r="F463" t="s">
-        <v>662</v>
-      </c>
-      <c r="K463">
-        <v>0.6</v>
+        <v>669</v>
+      </c>
+      <c r="K463" t="s">
+        <v>649</v>
       </c>
       <c r="L463" t="s">
         <v>649</v>
+      </c>
+      <c r="M463" t="s">
+        <v>649</v>
+      </c>
+      <c r="N463">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="464" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
@@ -19443,6 +19836,12 @@
       <c r="L464">
         <v>2.7</v>
       </c>
+      <c r="M464">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N464" s="3">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="465" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
@@ -19460,10 +19859,19 @@
       <c r="E465" t="s">
         <v>460</v>
       </c>
+      <c r="F465" t="s">
+        <v>670</v>
+      </c>
       <c r="K465">
         <v>1.3</v>
       </c>
-      <c r="L465">
+      <c r="L465" t="s">
+        <v>649</v>
+      </c>
+      <c r="M465">
+        <v>1.3</v>
+      </c>
+      <c r="N465">
         <v>1.7</v>
       </c>
     </row>
@@ -19489,6 +19897,12 @@
       <c r="L466">
         <v>8.3000000000000007</v>
       </c>
+      <c r="M466">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="N466">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="467" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
@@ -19512,6 +19926,12 @@
       <c r="L467">
         <v>2.2999999999999998</v>
       </c>
+      <c r="M467">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N467">
+        <v>5.0999999999999996</v>
+      </c>
     </row>
     <row r="468" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
@@ -19765,7 +20185,7 @@
         <v>460</v>
       </c>
       <c r="F476" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K476">
         <v>0.8</v>
@@ -19831,6 +20251,12 @@
       <c r="L478">
         <v>2</v>
       </c>
+      <c r="M478">
+        <v>2</v>
+      </c>
+      <c r="N478">
+        <v>2</v>
+      </c>
     </row>
     <row r="479" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
@@ -19854,6 +20280,12 @@
       <c r="L479">
         <v>3.3</v>
       </c>
+      <c r="M479">
+        <v>3.7</v>
+      </c>
+      <c r="N479">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="480" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
@@ -19877,6 +20309,12 @@
       <c r="L480">
         <v>1.9</v>
       </c>
+      <c r="M480">
+        <v>2.6</v>
+      </c>
+      <c r="N480">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="481" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
@@ -19895,12 +20333,18 @@
         <v>460</v>
       </c>
       <c r="F481" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K481" t="s">
         <v>649</v>
       </c>
       <c r="L481" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="M481" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="N481" s="3" t="s">
         <v>649</v>
       </c>
     </row>
@@ -19926,6 +20370,12 @@
       <c r="L482">
         <v>2.2999999999999998</v>
       </c>
+      <c r="M482">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N482">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="483" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
@@ -20239,6 +20689,12 @@
       <c r="L493">
         <v>1.9</v>
       </c>
+      <c r="M493">
+        <v>2.1</v>
+      </c>
+      <c r="N493">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="494" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
@@ -20262,6 +20718,12 @@
       <c r="L494">
         <v>1.5</v>
       </c>
+      <c r="M494">
+        <v>2.7</v>
+      </c>
+      <c r="N494">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="495" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
@@ -20285,6 +20747,12 @@
       <c r="L495">
         <v>1.8</v>
       </c>
+      <c r="M495">
+        <v>1.7</v>
+      </c>
+      <c r="N495">
+        <v>2</v>
+      </c>
     </row>
     <row r="496" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
@@ -20308,6 +20776,12 @@
       <c r="L496">
         <v>5.9</v>
       </c>
+      <c r="M496">
+        <v>9.9</v>
+      </c>
+      <c r="N496">
+        <v>10.1</v>
+      </c>
     </row>
     <row r="497" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
@@ -20331,6 +20805,12 @@
       <c r="L497">
         <v>2.4</v>
       </c>
+      <c r="M497">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N497">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="498" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
@@ -20647,6 +21127,12 @@
       <c r="L508">
         <v>1.4</v>
       </c>
+      <c r="M508">
+        <v>1.5</v>
+      </c>
+      <c r="N508">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="509" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
@@ -20670,6 +21156,12 @@
       <c r="L509">
         <v>5.9</v>
       </c>
+      <c r="M509">
+        <v>7.3</v>
+      </c>
+      <c r="N509">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="510" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
@@ -20693,6 +21185,12 @@
       <c r="L510">
         <v>6.2</v>
       </c>
+      <c r="M510">
+        <v>7</v>
+      </c>
+      <c r="N510">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="511" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
@@ -20716,6 +21214,12 @@
       <c r="L511">
         <v>1</v>
       </c>
+      <c r="M511">
+        <v>1</v>
+      </c>
+      <c r="N511">
+        <v>1</v>
+      </c>
     </row>
     <row r="512" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
@@ -20739,6 +21243,12 @@
       <c r="L512">
         <v>1.3</v>
       </c>
+      <c r="M512">
+        <v>1.3</v>
+      </c>
+      <c r="N512">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="513" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
@@ -21055,6 +21565,12 @@
       <c r="L523">
         <v>0.5</v>
       </c>
+      <c r="M523">
+        <v>0.6</v>
+      </c>
+      <c r="N523">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="524" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
@@ -21078,6 +21594,12 @@
       <c r="L524">
         <v>2.2000000000000002</v>
       </c>
+      <c r="M524">
+        <v>2.9</v>
+      </c>
+      <c r="N524">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="525" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
@@ -21101,6 +21623,12 @@
       <c r="L525">
         <v>4.5999999999999996</v>
       </c>
+      <c r="M525">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N525">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
     <row r="526" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
@@ -21124,6 +21652,12 @@
       <c r="L526">
         <v>1.5</v>
       </c>
+      <c r="M526">
+        <v>1.8</v>
+      </c>
+      <c r="N526">
+        <v>3.3</v>
+      </c>
     </row>
     <row r="527" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
@@ -21149,6 +21683,12 @@
       </c>
       <c r="L527">
         <v>1.1000000000000001</v>
+      </c>
+      <c r="M527">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N527">
+        <v>1.3</v>
       </c>
     </row>
     <row r="528" spans="1:14" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>